<commit_message>
creacion ticket parquedero v1.0.0
</commit_message>
<xml_diff>
--- a/bd_cinecolombia/Data/DATA_PARA_CARGAR.xlsx
+++ b/bd_cinecolombia/Data/DATA_PARA_CARGAR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCC\UCC_CreacionBD\bd_cinecolombia\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572F1235-9AF0-4837-9B76-D85BA7F84FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCC81E3-56A7-4010-9B84-282920AF5F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{42B65FB2-2B7F-49E6-A427-49DEDB5C9C54}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{42B65FB2-2B7F-49E6-A427-49DEDB5C9C54}"/>
   </bookViews>
   <sheets>
     <sheet name="PAIS" sheetId="2" r:id="rId1"/>
@@ -7965,8 +7965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6727EAFB-DED0-4134-85C0-58482A1E3CDB}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8496,8 +8496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4F9882-1464-4B41-B6B0-681DD22797E1}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>